<commit_message>
Began refactoring individual library parser and tests
</commit_message>
<xml_diff>
--- a/JamBio/Project_Storage/WO-TRANSFER/Sample_Sheet/Sample_Submission_Sheet_Indiv.xlsx
+++ b/JamBio/Project_Storage/WO-TRANSFER/Sample_Sheet/Sample_Submission_Sheet_Indiv.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Pooled Libraries" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Individual Libraries" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Individual Libraries" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Pooled Libraries" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t xml:space="preserve">General Information</t>
   </si>
@@ -57,6 +57,9 @@
     <t xml:space="preserve">Project ID:</t>
   </si>
   <si>
+    <t xml:space="preserve">Individual Libraries</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sequencing Information</t>
   </si>
   <si>
@@ -73,119 +76,6 @@
   </si>
   <si>
     <t xml:space="preserve">Additional Notes:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pooled Libraries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instructions: Please fill this section if you are submitting one or more pooled libaries. The Tube ID is the identifier on the physical container the material is submitted in. The Pool Name is the identifier for your library, this may be different or identical to the Tube ID. The Individual Library ID refers to a unique library with a unique index or indexes contained within a pool.
-Please fill out the Pool Information table with information about each tube submitted - there should be one row per tube. This is higher level information about the pool.
-Please complete the Indexing Information table for every library in every pool, this is the lower level information about each individual library. 
-An example is included below. Please fill out the the columns and rows for every sample, even if it seems redundant.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pool Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tube ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pool Names</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume (ul)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concentration (ng/ul)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Amount (ug)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantitation Method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buffer (TE or Water)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequencing Requirement (lanes)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pool1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qubit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indexing Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pool Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual Library ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample Preparation Kit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ave. Insert
- Size (bp)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ave. Library Size (bp)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i7 Index Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i7 Index Sequence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i5 Index Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i5 Index Sequence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Library Diversity (High or Low)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pool1_SAM42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nextera XT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATCGACTG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATCGATTCC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual Libraries</t>
   </si>
   <si>
     <r>
@@ -212,16 +102,171 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Tube ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual Library ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sample 
 Preparation 
 Kit</t>
   </si>
   <si>
+    <t xml:space="preserve">Volume (ul)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concentration (ng/ul)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ave. Insert
+ Size (bp)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ave. Library
 Size (bp)</t>
   </si>
   <si>
+    <t xml:space="preserve">i7 Index Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i7 Index Sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i5 Index Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i5 Index Sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library Diversity (High or Low)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAM42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nextera XT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATCGACTG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATCGATTCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nextera XT 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCCCCCCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL-G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGGGGGGG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAM2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nextera XT 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAAAAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTTTTTT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAM3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nextera XT 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTTTTT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pooled Libraries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instructions: Please fill this section if you are submitting one or more pooled libaries. The Tube ID is the identifier on the physical container the material is submitted in. The Pool Name is the identifier for your library, this may be different or identical to the Tube ID. The Individual Library ID refers to a unique library with a unique index or indexes contained within a pool.
+Please fill out the Pool Information table with information about each tube submitted - there should be one row per tube. This is higher level information about the pool.
+Please complete the Indexing Information table for every library in every pool, this is the lower level information about each individual library. 
+An example is included below. Please fill out the the columns and rows for every sample, even if it seems redundant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pool Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pool Names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Amount (ug)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantitation Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffer (TE or Water)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequencing Requirement (lanes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pool1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qubit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexing Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pool Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Preparation Kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ave. Library Size (bp)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pool1_SAM42</t>
   </si>
 </sst>
 </file>
@@ -231,7 +276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -253,20 +298,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -305,6 +336,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -320,6 +358,48 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -344,47 +424,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -406,7 +445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -472,6 +511,48 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
+      <right style="hair"/>
+      <top style="medium"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="medium"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="medium"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
       <right style="thin"/>
       <top style="medium"/>
       <bottom style="thin"/>
@@ -526,57 +607,8 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thick"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -600,302 +632,269 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="4" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="15" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="16" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="16" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="11" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="17" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="12" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="18" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="4" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="13" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="19" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="18" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="19" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="18" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="20" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="21" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="22" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="12" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="13" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="14" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 3" xfId="22" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -967,18 +966,18 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1253,10 +1252,14 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
-      <c r="B10" s="16"/>
+      <c r="B10" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="16" t="n">
+        <v>123456</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1306,7 +1309,7 @@
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -1336,16 +1339,16 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1424,7 +1427,7 @@
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
@@ -2477,7 +2480,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B10" type="list">
-      <formula1>"DNA,RNA,Pooled Libraries,Individual Libraries"</formula1>
+      <formula1>"Pooled Libraries,Individual Libraries"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2496,493 +2499,915 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M40"/>
+  <dimension ref="B1:M101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="16.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="21.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="20.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="23.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="23.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="19.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="20" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="20" width="19.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="20" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="20" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="20" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="20" width="14.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="20" width="12.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="20" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="20" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="20" width="14.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="14.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="21" t="s">
-        <v>17</v>
+      <c r="B1" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+    </row>
+    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+    </row>
+    <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+    </row>
+    <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+    </row>
+    <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="29" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="29" t="n">
+        <v>300</v>
+      </c>
+      <c r="H9" s="29" t="n">
+        <v>350</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="31" t="n">
+        <v>11</v>
+      </c>
+      <c r="F10" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="31" t="n">
+        <v>301</v>
+      </c>
+      <c r="H10" s="31" t="n">
+        <v>351</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="31" t="n">
+        <v>12</v>
+      </c>
+      <c r="F11" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="31" t="n">
+        <v>302</v>
+      </c>
+      <c r="H11" s="31" t="n">
+        <v>352</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="L11" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="31" t="n">
+        <v>13</v>
+      </c>
+      <c r="F12" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="31" t="n">
+        <v>302</v>
+      </c>
+      <c r="H12" s="31" t="n">
+        <v>353</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:I6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M125"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="20.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="33" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="33" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="33" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="33" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="33" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="33" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="33" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="33" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="33" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="33" width="14.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="33" width="12.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="33" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="33" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="33" width="14.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="34" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
+      <c r="A3" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
     </row>
     <row r="7" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
     </row>
     <row r="9" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
     </row>
     <row r="10" customFormat="false" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="25" t="s">
-        <v>20</v>
+      <c r="B10" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="39.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="27" t="s">
+      <c r="B12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="E12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>29</v>
+      <c r="F12" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="30" t="n">
+      <c r="B13" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="31" t="n">
+      <c r="C13" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="44" t="n">
         <v>10</v>
       </c>
-      <c r="E13" s="31" t="n">
+      <c r="E13" s="44" t="n">
         <v>50</v>
       </c>
-      <c r="F13" s="31" t="n">
+      <c r="F13" s="44" t="n">
         <v>0.5</v>
       </c>
-      <c r="G13" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="32" t="n">
+      <c r="G13" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="45" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="35"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="49"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="35"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="49"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="35"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="35"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="35"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="35"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="49"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="36"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="35"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="49"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="36"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="35"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="49"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="36"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="35"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="49"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="36"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="35"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="49"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="36"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="35"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="49"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="36"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="35"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="49"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="36"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="35"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="49"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="36"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="35"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="49"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="36"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="35"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="36"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="35"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="49"/>
     </row>
     <row r="30" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="37"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="53"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="25" t="s">
-        <v>34</v>
+      <c r="B33" s="38" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="40.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="G35" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="I35" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="K35" s="57" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="59" t="n">
+        <v>300</v>
+      </c>
+      <c r="F36" s="59" t="n">
+        <v>350</v>
+      </c>
+      <c r="G36" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="I36" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="J36" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="K36" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="G35" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="H35" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="I35" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="J35" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="K35" s="29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="31" t="n">
-        <v>300</v>
-      </c>
-      <c r="F36" s="31" t="n">
-        <v>350</v>
-      </c>
-      <c r="G36" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="H36" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="I36" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="J36" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="K36" s="32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="36"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
-      <c r="K37" s="43"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="36"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="43"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="36"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="42"/>
-      <c r="K39" s="43"/>
-    </row>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3068,6 +3493,23 @@
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:J9"/>
@@ -3080,466 +3522,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B1:M23"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="14.34"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-    </row>
-    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-    </row>
-    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-    </row>
-    <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-    </row>
-    <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-    </row>
-    <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="50" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="54" t="n">
-        <v>10</v>
-      </c>
-      <c r="F9" s="54" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="53" t="n">
-        <v>300</v>
-      </c>
-      <c r="H9" s="54" t="n">
-        <v>350</v>
-      </c>
-      <c r="I9" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="L9" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="M9" s="55" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="56"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="43"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="56"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="43"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="56"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="61"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="56"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="61"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="56"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="61"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="56"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="61"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="62"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="61"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="62"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="61"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="62"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="61"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="62"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="61"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="64"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="61"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="62"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="66"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="67"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="65"/>
-      <c r="M22" s="66"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:I6"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>